<commit_message>
fix test_calc_reaction_rates(); fix docstrings
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/test_submodel_no_shared_species.xlsx
+++ b/tests/submodels/fixtures/test_submodel_no_shared_species.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-8560" yWindow="24500" windowWidth="22500" windowHeight="12040" tabRatio="993" activeTab="8"/>
+    <workbookView xWindow="-8560" yWindow="24500" windowWidth="22500" windowHeight="12040" tabRatio="993" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -1858,16 +1858,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1:I1"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="20" customWidth="1"/>
+    <col min="1" max="1" width="12" style="20" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" style="20" customWidth="1"/>
     <col min="3" max="3" width="10.5" style="20" customWidth="1"/>
     <col min="4" max="4" width="46.83203125" style="20" customWidth="1"/>
@@ -2092,11 +2092,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2:E7"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2558,11 +2558,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6359,14 +6359,15 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2:D8"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" style="20" customWidth="1"/>
     <col min="2" max="2" width="5.6640625" style="20" customWidth="1"/>
-    <col min="3" max="4" width="11" style="20" customWidth="1"/>
+    <col min="3" max="3" width="11" style="20" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" style="20" customWidth="1"/>
     <col min="6" max="6" width="17.1640625" style="20" customWidth="1"/>
     <col min="7" max="7" width="7.83203125" style="20" customWidth="1"/>

</xml_diff>

<commit_message>
make self.multialgorithm_simulation.simulation_submodels a dict; instantiate a submodel with framework of X_deterministic_simulation_algorithm as a DeterministicSimulationAlgorithmSubmodel; test DeterministicSimulationAlgorithmSubmodel; fix test_submodel_no_shared_species.xlsx
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/test_submodel_no_shared_species.xlsx
+++ b/tests/submodels/fixtures/test_submodel_no_shared_species.xlsx
@@ -9,7 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-8560" yWindow="24500" windowWidth="22500" windowHeight="12040" tabRatio="993" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="-11500" yWindow="24500" windowWidth="22500" windowHeight="12040" tabRatio="993" firstSheet="9" activeTab="16"/>
+    <workbookView xWindow="-13740" yWindow="29840" windowWidth="19960" windowHeight="7080" tabRatio="500" firstSheet="4" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -52,20 +53,20 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">'!References'!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'!Species types'!$A$2:$K$8</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="5">[1]Compartments!$A$2:$G$4</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="16">[4]Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="16">[2]Parameters!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="11">[3]Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="21">[5]References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="6">'[2]Species types'!$A$2:$K$7</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="21">[4]References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="5">[1]Compartments!$A$2:$G$4</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="16">[4]Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="16">[2]Parameters!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="11">[3]Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="21">[5]References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="6">'[2]Species types'!$A$2:$K$7</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="21">[4]References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="5">[1]Compartments!$A$2:$G$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="16">[4]Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="16">[2]Parameters!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="11">[3]Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="21">[5]References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'[2]Species types'!$A$2:$K$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="21">[4]References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -1141,7 +1142,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Species types"/>
+      <sheetName val="Parameters"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1167,7 +1168,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Parameters"/>
+      <sheetName val="References"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1180,7 +1181,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="References"/>
+      <sheetName val="Species types"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1453,6 +1454,7 @@
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A19:A21"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1724,6 +1726,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1782,6 +1785,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1864,19 +1868,25 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1">
+      <selection activeCell="A6" sqref="A6:A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" style="20" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="20" customWidth="1"/>
-    <col min="4" max="4" width="46.83203125" style="20" customWidth="1"/>
-    <col min="5" max="6" width="8.1640625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="42" style="20" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="20" customWidth="1"/>
+    <col min="6" max="6" width="8.1640625" style="20" customWidth="1"/>
     <col min="7" max="7" width="7.5" style="15" customWidth="1"/>
     <col min="8" max="8" width="7.6640625" style="15" customWidth="1"/>
     <col min="9" max="9" width="37.83203125" style="20" customWidth="1"/>
     <col min="10" max="10" width="8.83203125" style="20" customWidth="1"/>
-    <col min="11" max="1027" width="8.83203125" style="15" customWidth="1"/>
+    <col min="11" max="12" width="8.83203125" style="15" customWidth="1"/>
+    <col min="13" max="13" width="37.33203125" style="15" customWidth="1"/>
+    <col min="14" max="1027" width="8.83203125" style="15" customWidth="1"/>
     <col min="1028" max="1028" width="9" style="15" customWidth="1"/>
     <col min="1029" max="16384" width="9" style="15"/>
   </cols>
@@ -1904,7 +1914,7 @@
       <c r="M2" s="16"/>
       <c r="N2" s="16"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="28" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>28</v>
       </c>
@@ -2092,12 +2102,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2276,6 +2287,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" sqref="A1:XFD1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2365,6 +2377,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2451,6 +2464,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2558,12 +2572,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2709,6 +2724,9 @@
       <c r="C9" s="20" t="s">
         <v>215</v>
       </c>
+      <c r="D9" s="20">
+        <v>2</v>
+      </c>
       <c r="F9" s="20" t="s">
         <v>160</v>
       </c>
@@ -2788,6 +2806,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="N13" sqref="N13"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2846,6 +2865,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="V1" sqref="V1:V1048576"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2970,6 +2990,7 @@
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A8" sqref="A8:XFD10"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3086,6 +3107,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="F5" sqref="A2:F5"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3147,6 +3169,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="N2" sqref="N2"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3266,6 +3289,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3353,6 +3377,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3418,6 +3443,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3496,6 +3522,7 @@
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B2" sqref="B1:B1048576"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3565,6 +3592,7 @@
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A6" sqref="A5:XFD6"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3637,12 +3665,18 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="7" width="8.83203125" style="14" customWidth="1"/>
+    <col min="1" max="1" width="15" style="14" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="8.83203125" style="14" customWidth="1"/>
     <col min="8" max="1026" width="8.83203125" style="18" customWidth="1"/>
     <col min="1027" max="1027" width="9" style="18" customWidth="1"/>
     <col min="1028" max="16384" width="9" style="18"/>
@@ -3713,11 +3747,12 @@
   <dimension ref="A1:AMR5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M1" sqref="M1:P4"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5849,7 +5884,7 @@
       <c r="AMQ3" s="16"/>
       <c r="AMR3" s="16"/>
     </row>
-    <row r="4" spans="1:1032" ht="252" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1032" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
         <v>82</v>
       </c>
@@ -5902,7 +5937,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:1032" ht="168" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1032" ht="59" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
         <v>87</v>
       </c>
@@ -5973,6 +6008,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6178,6 +6214,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6355,12 +6392,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>